<commit_message>
Also write username to db
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Vorname</t>
   </si>
@@ -25,6 +25,12 @@
   </si>
   <si>
     <t>Karte</t>
+  </si>
+  <si>
+    <t>Hans</t>
+  </si>
+  <si>
+    <t>Wurst</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,6 +389,17 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new columns to example excel file
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Vorname</t>
   </si>
@@ -31,6 +31,24 @@
   </si>
   <si>
     <t>Wurst</t>
+  </si>
+  <si>
+    <t>AHV-Nr</t>
+  </si>
+  <si>
+    <t>Grad</t>
+  </si>
+  <si>
+    <t>Funktion</t>
+  </si>
+  <si>
+    <t>756.9217.0769.85</t>
+  </si>
+  <si>
+    <t>Sdt</t>
+  </si>
+  <si>
+    <t>Stabsassistent</t>
   </si>
 </sst>
 </file>
@@ -369,41 +387,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
         <v>1234</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>